<commit_message>
feat: add dropdown for DM fee type in Excel template v5
- Cell E11 now has dropdown: "Фикс" or "комиссия %"
- Default value: Фикс
- Replaces previous free-text "фикс. сумма"

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/validation_data/template_quote_input_v5.xlsx
+++ b/validation_data/template_quote_input_v5.xlsx
@@ -53,7 +53,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -67,16 +67,46 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -470,16 +500,21 @@
           <t>НАСТРОЙКИ КОТИРОВКИ</t>
         </is>
       </c>
+      <c r="B1" s="5" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>УСЛОВИЯ ОПЛАТЫ</t>
         </is>
       </c>
+      <c r="E1" s="6" t="n"/>
+      <c r="F1" s="5" t="n"/>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ЛОГИСТИКА</t>
         </is>
       </c>
+      <c r="I1" s="6" t="n"/>
+      <c r="J1" s="5" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -650,6 +685,8 @@
           <t>БРОКЕРСКИЕ УСЛУГИ</t>
         </is>
       </c>
+      <c r="I6" s="6" t="n"/>
+      <c r="J6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -724,6 +761,8 @@
           <t>ВОЗНАГРАЖДЕНИЕ ЛПР</t>
         </is>
       </c>
+      <c r="E10" s="6" t="n"/>
+      <c r="F10" s="5" t="n"/>
       <c r="H10" s="2" t="inlineStr">
         <is>
           <t>Расходы на СВХ</t>
@@ -746,9 +785,10 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>фикс. сумма</t>
-        </is>
-      </c>
+          <t>Фикс</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="n"/>
       <c r="H11" s="2" t="inlineStr">
         <is>
           <t>Разреш. документы</t>
@@ -797,6 +837,17 @@
           <t>ТОВАРЫ</t>
         </is>
       </c>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
+      <c r="D14" s="6" t="n"/>
+      <c r="E14" s="6" t="n"/>
+      <c r="F14" s="6" t="n"/>
+      <c r="G14" s="6" t="n"/>
+      <c r="H14" s="6" t="n"/>
+      <c r="I14" s="6" t="n"/>
+      <c r="J14" s="6" t="n"/>
+      <c r="K14" s="6" t="n"/>
+      <c r="L14" s="5" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
@@ -1250,7 +1301,7 @@
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D10:F10"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"МАСТЕР БЭРИНГ ООО,ЦМТО1 ООО,РАД РЕСУРС ООО,TEXCEL OTOMOTİV TİCARET LİMİTED ŞİRKETİ,GESTUS DIŞ TİCARET LİMİTED ŞİRKETİ,UPDOOR Limited"</formula1>
     </dataValidation>
@@ -1269,6 +1320,9 @@
     <dataValidation sqref="E11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"% от суммы,фикс. сумма"</formula1>
     </dataValidation>
+    <dataValidation sqref="E11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Неверный тип" error="Выберите тип из списка" promptTitle="Тип" prompt="Выберите тип вознаграждения" type="list">
+      <formula1>"Фикс,комиссия %"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>